<commit_message>
Keywords - collect column
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clib_\OneDrive\Desktop\SHAPER\PROJECTS\FIVERR\twitter-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721B24A9-29C5-47AD-98A6-52681AA6DEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D6C94B-123D-4A9E-A92F-763B7DE450DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>keywords</t>
   </si>
@@ -52,6 +63,15 @@
   </si>
   <si>
     <t>Embalagem alimento</t>
+  </si>
+  <si>
+    <t>collect</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Rotulo alimento</t>
   </si>
 </sst>
 </file>
@@ -369,61 +389,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
keywords - Since + Until Filter
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clib_\OneDrive\Desktop\SHAPER\PROJECTS\FIVERR\twitter-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D6C94B-123D-4A9E-A92F-763B7DE450DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D76CB6-38AE-4FC1-B89A-A7E1D6CAE019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>keywords</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Rotulo alimento</t>
+  </si>
+  <si>
+    <t>since</t>
+  </si>
+  <si>
+    <t>until</t>
   </si>
 </sst>
 </file>
@@ -87,12 +93,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,8 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,95 +410,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44113</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>